<commit_message>
Clean up telecom billing anomaly detection system
</commit_message>
<xml_diff>
--- a/data/Anomalies/Anomalies_10-3-2025.xlsx
+++ b/data/Anomalies/Anomalies_10-3-2025.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Anomalies" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +57,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -491,52 +495,52 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
+          <t>Rolling_Avg</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Active_vs_Avg</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Pct_Change_Active_vs_Avg</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>MoM_Change</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Pct_Change_MoM</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Drop_to_0</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>New_Code</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Active_vs_Avg_z</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Anomaly</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>Billing Code Description</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Rolling_Avg</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Active_vs_Avg</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Pct_Change_Active_vs_Avg</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>MoM_Change</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>Pct_Change_MoM</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>Drop_to_0</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>New_Code</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Active_vs_Avg_z</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>Anomaly</t>
         </is>
       </c>
     </row>
@@ -560,55 +564,55 @@
           <t>SEC009</t>
         </is>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" s="2" t="n">
         <v>960503.04</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="2" t="n">
         <v>1310107.37</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2" s="2" t="n">
         <v>1762359.53</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2" s="2" t="n">
         <v>1942642.28</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2" s="2" t="n">
         <v>3153079.5</v>
       </c>
-      <c r="K2" t="n">
+      <c r="K2" s="2" t="n">
         <v>4058787.42</v>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="L2" s="2" t="n">
+        <v>1825738.344</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>2233049.076</v>
+      </c>
+      <c r="N2" s="3" t="n">
+        <v>1.223093705260977</v>
+      </c>
+      <c r="O2" s="2" t="n">
+        <v>3098284.38</v>
+      </c>
+      <c r="P2" s="3" t="n">
+        <v>3.225689301306115</v>
+      </c>
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="n">
+        <v>1.293865501036378</v>
+      </c>
+      <c r="T2" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" t="inlineStr">
         <is>
           <t>SIM card replacement charge</t>
         </is>
-      </c>
-      <c r="M2" t="n">
-        <v>1825738.344</v>
-      </c>
-      <c r="N2" t="n">
-        <v>2233049.076</v>
-      </c>
-      <c r="O2" t="n">
-        <v>1.223093705260977</v>
-      </c>
-      <c r="P2" t="n">
-        <v>3098284.38</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>3.225689301306115</v>
-      </c>
-      <c r="R2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T2" t="n">
-        <v>1.293865501036378</v>
-      </c>
-      <c r="U2" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -631,55 +635,55 @@
           <t>SEC039</t>
         </is>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" s="2" t="n">
         <v>2293543.36</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="2" t="n">
         <v>2746374.64</v>
       </c>
-      <c r="H3" t="n">
+      <c r="H3" s="2" t="n">
         <v>2696698.51</v>
       </c>
-      <c r="I3" t="n">
+      <c r="I3" s="2" t="n">
         <v>2868717.18</v>
       </c>
-      <c r="J3" t="n">
+      <c r="J3" s="2" t="n">
         <v>3348737.68</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3" s="2" t="n">
         <v>4202212.9</v>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="L3" s="2" t="n">
+        <v>2790814.274</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>1411398.626</v>
+      </c>
+      <c r="N3" s="3" t="n">
+        <v>0.5057300441483983</v>
+      </c>
+      <c r="O3" s="2" t="n">
+        <v>1908669.540000001</v>
+      </c>
+      <c r="P3" s="3" t="n">
+        <v>0.832192481418795</v>
+      </c>
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.5586398920232797</v>
+      </c>
+      <c r="T3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" t="inlineStr">
         <is>
           <t>One-time Voicemail transcription fee</t>
         </is>
-      </c>
-      <c r="M3" t="n">
-        <v>2790814.274</v>
-      </c>
-      <c r="N3" t="n">
-        <v>1411398.626</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0.5057300441483983</v>
-      </c>
-      <c r="P3" t="n">
-        <v>1908669.540000001</v>
-      </c>
-      <c r="Q3" t="n">
-        <v>0.832192481418795</v>
-      </c>
-      <c r="R3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" t="b">
-        <v>0</v>
-      </c>
-      <c r="T3" t="n">
-        <v>0.5586398920232797</v>
-      </c>
-      <c r="U3" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -702,55 +706,55 @@
           <t>SEC025</t>
         </is>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" s="2" t="n">
         <v>7012977.91</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" s="2" t="n">
         <v>7028800.38</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4" s="2" t="n">
         <v>7488157.86</v>
       </c>
-      <c r="I4" t="n">
+      <c r="I4" s="2" t="n">
         <v>7546408.48</v>
       </c>
-      <c r="J4" t="n">
+      <c r="J4" s="2" t="n">
         <v>8079327.93</v>
       </c>
-      <c r="K4" t="n">
+      <c r="K4" s="2" t="n">
         <v>5020830.59</v>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="L4" s="2" t="n">
+        <v>7431134.512</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>-2410303.922</v>
+      </c>
+      <c r="N4" s="3" t="n">
+        <v>-0.324352078152774</v>
+      </c>
+      <c r="O4" s="2" t="n">
+        <v>-1992147.32</v>
+      </c>
+      <c r="P4" s="3" t="n">
+        <v>-0.2840658199078799</v>
+      </c>
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-2.861079020465857</v>
+      </c>
+      <c r="T4" t="b">
+        <v>1</v>
+      </c>
+      <c r="U4" t="inlineStr">
         <is>
           <t>Roaming charge outside of coverage area</t>
         </is>
-      </c>
-      <c r="M4" t="n">
-        <v>7431134.512</v>
-      </c>
-      <c r="N4" t="n">
-        <v>-2410303.922</v>
-      </c>
-      <c r="O4" t="n">
-        <v>-0.324352078152774</v>
-      </c>
-      <c r="P4" t="n">
-        <v>-1992147.32</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>-0.2840658199078799</v>
-      </c>
-      <c r="R4" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4" t="b">
-        <v>0</v>
-      </c>
-      <c r="T4" t="n">
-        <v>-2.861079020465857</v>
-      </c>
-      <c r="U4" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -773,55 +777,55 @@
           <t>SEC009</t>
         </is>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="2" t="n">
         <v>1216313.23</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="2" t="n">
         <v>1389736.26</v>
       </c>
-      <c r="H5" t="n">
+      <c r="H5" s="2" t="n">
         <v>1728353.57</v>
       </c>
-      <c r="I5" t="n">
+      <c r="I5" s="2" t="n">
         <v>1427858.13</v>
       </c>
-      <c r="J5" t="n">
+      <c r="J5" s="2" t="n">
         <v>1961327.86</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K5" s="2" t="n">
         <v>3928316.12</v>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="L5" s="2" t="n">
+        <v>1544717.81</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>2383598.31</v>
+      </c>
+      <c r="N5" s="3" t="n">
+        <v>1.54306391404913</v>
+      </c>
+      <c r="O5" s="2" t="n">
+        <v>2712002.89</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>2.22969118735969</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1.428579298435388</v>
+      </c>
+      <c r="T5" t="b">
+        <v>1</v>
+      </c>
+      <c r="U5" t="inlineStr">
         <is>
           <t>SIM card replacement charge</t>
         </is>
-      </c>
-      <c r="M5" t="n">
-        <v>1544717.81</v>
-      </c>
-      <c r="N5" t="n">
-        <v>2383598.31</v>
-      </c>
-      <c r="O5" t="n">
-        <v>1.54306391404913</v>
-      </c>
-      <c r="P5" t="n">
-        <v>2712002.89</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>2.22969118735969</v>
-      </c>
-      <c r="R5" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5" t="n">
-        <v>1.428579298435388</v>
-      </c>
-      <c r="U5" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -844,55 +848,55 @@
           <t>SEC037</t>
         </is>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="2" t="n">
         <v>2133515.77</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="2" t="n">
         <v>2354277.14</v>
       </c>
-      <c r="H6" t="n">
+      <c r="H6" s="2" t="n">
         <v>2834679.29</v>
       </c>
-      <c r="I6" t="n">
+      <c r="I6" s="2" t="n">
         <v>2773839.65</v>
       </c>
-      <c r="J6" t="n">
+      <c r="J6" s="2" t="n">
         <v>3771338.89</v>
       </c>
-      <c r="K6" t="n">
+      <c r="K6" s="2" t="n">
         <v>4383240.41</v>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="L6" s="2" t="n">
+        <v>2773530.148</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>1609710.262</v>
+      </c>
+      <c r="N6" s="3" t="n">
+        <v>0.5803831853642429</v>
+      </c>
+      <c r="O6" s="2" t="n">
+        <v>2249724.64</v>
+      </c>
+      <c r="P6" s="3" t="n">
+        <v>1.054468249840966</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.7360922300004376</v>
+      </c>
+      <c r="T6" t="b">
+        <v>1</v>
+      </c>
+      <c r="U6" t="inlineStr">
         <is>
           <t>Non-returned equipment charge</t>
         </is>
-      </c>
-      <c r="M6" t="n">
-        <v>2773530.148</v>
-      </c>
-      <c r="N6" t="n">
-        <v>1609710.262</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.5803831853642429</v>
-      </c>
-      <c r="P6" t="n">
-        <v>2249724.64</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>1.054468249840966</v>
-      </c>
-      <c r="R6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.7360922300004376</v>
-      </c>
-      <c r="U6" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -915,55 +919,55 @@
           <t>SEC034</t>
         </is>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="2" t="n">
         <v>1020013.57</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="2" t="n">
         <v>1190263.24</v>
       </c>
-      <c r="H7" t="n">
+      <c r="H7" s="2" t="n">
         <v>1723887.82</v>
       </c>
-      <c r="I7" t="n">
+      <c r="I7" s="2" t="n">
         <v>2142792.99</v>
       </c>
-      <c r="J7" t="n">
+      <c r="J7" s="2" t="n">
         <v>2762853.78</v>
       </c>
-      <c r="K7" t="n">
+      <c r="K7" s="2" t="n">
         <v>2734906.8</v>
       </c>
-      <c r="L7" t="inlineStr">
+      <c r="L7" s="2" t="n">
+        <v>1767962.28</v>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>966944.5199999998</v>
+      </c>
+      <c r="N7" s="3" t="n">
+        <v>0.5469259898463443</v>
+      </c>
+      <c r="O7" s="2" t="n">
+        <v>1714893.23</v>
+      </c>
+      <c r="P7" s="3" t="n">
+        <v>1.681245505390678</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.1609354414722912</v>
+      </c>
+      <c r="T7" t="b">
+        <v>1</v>
+      </c>
+      <c r="U7" t="inlineStr">
         <is>
           <t>Installation fee for home wireless equipment</t>
         </is>
-      </c>
-      <c r="M7" t="n">
-        <v>1767962.28</v>
-      </c>
-      <c r="N7" t="n">
-        <v>966944.5199999998</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.5469259898463443</v>
-      </c>
-      <c r="P7" t="n">
-        <v>1714893.23</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>1.681245505390678</v>
-      </c>
-      <c r="R7" t="b">
-        <v>0</v>
-      </c>
-      <c r="S7" t="b">
-        <v>0</v>
-      </c>
-      <c r="T7" t="n">
-        <v>0.1609354414722912</v>
-      </c>
-      <c r="U7" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -986,55 +990,55 @@
           <t>SEC033</t>
         </is>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="2" t="n">
         <v>2614713.47</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="2" t="n">
         <v>2650340.66</v>
       </c>
-      <c r="H8" t="n">
+      <c r="H8" s="2" t="n">
         <v>3016154.79</v>
       </c>
-      <c r="I8" t="n">
+      <c r="I8" s="2" t="n">
         <v>3205221.3</v>
       </c>
-      <c r="J8" t="n">
+      <c r="J8" s="2" t="n">
         <v>3076657</v>
       </c>
-      <c r="K8" t="n">
+      <c r="K8" s="2" t="n">
         <v>1270448.01</v>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="L8" s="2" t="n">
+        <v>2912617.444</v>
+      </c>
+      <c r="M8" s="2" t="n">
+        <v>-1642169.434</v>
+      </c>
+      <c r="N8" s="3" t="n">
+        <v>-0.5638122635648131</v>
+      </c>
+      <c r="O8" s="2" t="n">
+        <v>-1344265.46</v>
+      </c>
+      <c r="P8" s="3" t="n">
+        <v>-0.5141157818718852</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>-2.173740327054608</v>
+      </c>
+      <c r="T8" t="b">
+        <v>1</v>
+      </c>
+      <c r="U8" t="inlineStr">
         <is>
           <t>One-time charge for mobile insurance</t>
         </is>
-      </c>
-      <c r="M8" t="n">
-        <v>2912617.444</v>
-      </c>
-      <c r="N8" t="n">
-        <v>-1642169.434</v>
-      </c>
-      <c r="O8" t="n">
-        <v>-0.5638122635648131</v>
-      </c>
-      <c r="P8" t="n">
-        <v>-1344265.46</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>-0.5141157818718852</v>
-      </c>
-      <c r="R8" t="b">
-        <v>0</v>
-      </c>
-      <c r="S8" t="b">
-        <v>0</v>
-      </c>
-      <c r="T8" t="n">
-        <v>-2.173740327054608</v>
-      </c>
-      <c r="U8" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -1057,55 +1061,55 @@
           <t>SEC017</t>
         </is>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="2" t="n">
         <v>1727598.37</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="2" t="n">
         <v>1859058.04</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H9" s="2" t="n">
         <v>2195192.51</v>
       </c>
-      <c r="I9" t="n">
+      <c r="I9" s="2" t="n">
         <v>3070237.18</v>
       </c>
-      <c r="J9" t="n">
+      <c r="J9" s="2" t="n">
         <v>2776702.78</v>
       </c>
-      <c r="K9" t="n">
+      <c r="K9" s="2" t="n">
         <v>4185603.7</v>
       </c>
-      <c r="L9" t="inlineStr">
+      <c r="L9" s="2" t="n">
+        <v>2325757.776</v>
+      </c>
+      <c r="M9" s="2" t="n">
+        <v>1859845.924000001</v>
+      </c>
+      <c r="N9" s="3" t="n">
+        <v>0.7996730971695141</v>
+      </c>
+      <c r="O9" s="2" t="n">
+        <v>2458005.33</v>
+      </c>
+      <c r="P9" s="3" t="n">
+        <v>1.422787479244959</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>0</v>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.9599175129170902</v>
+      </c>
+      <c r="T9" t="b">
+        <v>1</v>
+      </c>
+      <c r="U9" t="inlineStr">
         <is>
           <t>Fee for non-returned leased device</t>
         </is>
-      </c>
-      <c r="M9" t="n">
-        <v>2325757.776</v>
-      </c>
-      <c r="N9" t="n">
-        <v>1859845.924000001</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.7996730971695141</v>
-      </c>
-      <c r="P9" t="n">
-        <v>2458005.33</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>1.422787479244959</v>
-      </c>
-      <c r="R9" t="b">
-        <v>0</v>
-      </c>
-      <c r="S9" t="b">
-        <v>0</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0.9599175129170902</v>
-      </c>
-      <c r="U9" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1128,55 +1132,55 @@
           <t>ACR040</t>
         </is>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="2" t="n">
         <v>1509121.89</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" s="2" t="n">
         <v>1201804.43</v>
       </c>
-      <c r="H10" t="n">
+      <c r="H10" s="2" t="n">
         <v>1929817.23</v>
       </c>
-      <c r="I10" t="n">
+      <c r="I10" s="2" t="n">
         <v>1683478.03</v>
       </c>
-      <c r="J10" t="n">
+      <c r="J10" s="2" t="n">
         <v>2957887.95</v>
       </c>
-      <c r="K10" t="n">
+      <c r="K10" s="2" t="n">
         <v>3427917.96</v>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="L10" s="2" t="n">
+        <v>1856421.906</v>
+      </c>
+      <c r="M10" s="2" t="n">
+        <v>1571496.054</v>
+      </c>
+      <c r="N10" s="3" t="n">
+        <v>0.8465188053000704</v>
+      </c>
+      <c r="O10" s="2" t="n">
+        <v>1918796.07</v>
+      </c>
+      <c r="P10" s="3" t="n">
+        <v>1.271465269117527</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.7018975620004949</v>
+      </c>
+      <c r="T10" t="b">
+        <v>1</v>
+      </c>
+      <c r="U10" t="inlineStr">
         <is>
           <t>Bundled service credit for partner plan</t>
         </is>
-      </c>
-      <c r="M10" t="n">
-        <v>1856421.906</v>
-      </c>
-      <c r="N10" t="n">
-        <v>1571496.054</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.8465188053000704</v>
-      </c>
-      <c r="P10" t="n">
-        <v>1918796.07</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>1.271465269117527</v>
-      </c>
-      <c r="R10" t="b">
-        <v>0</v>
-      </c>
-      <c r="S10" t="b">
-        <v>0</v>
-      </c>
-      <c r="T10" t="n">
-        <v>0.7018975620004949</v>
-      </c>
-      <c r="U10" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -1199,55 +1203,55 @@
           <t>ACR016</t>
         </is>
       </c>
-      <c r="F11" t="n">
+      <c r="F11" s="2" t="n">
         <v>2739491.18</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11" s="2" t="n">
         <v>3692677</v>
       </c>
-      <c r="H11" t="n">
+      <c r="H11" s="2" t="n">
         <v>4118944.95</v>
       </c>
-      <c r="I11" t="n">
+      <c r="I11" s="2" t="n">
         <v>4665970.85</v>
       </c>
-      <c r="J11" t="n">
+      <c r="J11" s="2" t="n">
         <v>4425820.19</v>
       </c>
-      <c r="K11" t="n">
+      <c r="K11" s="2" t="n">
         <v>6063719.29</v>
       </c>
-      <c r="L11" t="inlineStr">
+      <c r="L11" s="2" t="n">
+        <v>3928580.834</v>
+      </c>
+      <c r="M11" s="2" t="n">
+        <v>2135138.456</v>
+      </c>
+      <c r="N11" s="3" t="n">
+        <v>0.543488487629271</v>
+      </c>
+      <c r="O11" s="2" t="n">
+        <v>3324228.11</v>
+      </c>
+      <c r="P11" s="3" t="n">
+        <v>1.213447276001086</v>
+      </c>
+      <c r="Q11" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>1.206253554595711</v>
+      </c>
+      <c r="T11" t="b">
+        <v>1</v>
+      </c>
+      <c r="U11" t="inlineStr">
         <is>
           <t>Credit from multi-line family plan</t>
         </is>
-      </c>
-      <c r="M11" t="n">
-        <v>3928580.834</v>
-      </c>
-      <c r="N11" t="n">
-        <v>2135138.456</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.543488487629271</v>
-      </c>
-      <c r="P11" t="n">
-        <v>3324228.11</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>1.213447276001086</v>
-      </c>
-      <c r="R11" t="b">
-        <v>0</v>
-      </c>
-      <c r="S11" t="b">
-        <v>0</v>
-      </c>
-      <c r="T11" t="n">
-        <v>1.206253554595711</v>
-      </c>
-      <c r="U11" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -1270,55 +1274,55 @@
           <t>ACR035</t>
         </is>
       </c>
-      <c r="F12" t="n">
+      <c r="F12" s="2" t="n">
         <v>2783289.5</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12" s="2" t="n">
         <v>3625664.18</v>
       </c>
-      <c r="H12" t="n">
+      <c r="H12" s="2" t="n">
         <v>3070437.55</v>
       </c>
-      <c r="I12" t="n">
+      <c r="I12" s="2" t="n">
         <v>3465378.1</v>
       </c>
-      <c r="J12" t="n">
+      <c r="J12" s="2" t="n">
         <v>4679611.04</v>
       </c>
-      <c r="K12" t="n">
+      <c r="K12" s="2" t="n">
         <v>6274362.72</v>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="L12" s="2" t="n">
+        <v>3524876.074</v>
+      </c>
+      <c r="M12" s="2" t="n">
+        <v>2749486.646</v>
+      </c>
+      <c r="N12" s="3" t="n">
+        <v>0.7800236343855077</v>
+      </c>
+      <c r="O12" s="2" t="n">
+        <v>3491073.22</v>
+      </c>
+      <c r="P12" s="3" t="n">
+        <v>1.254297556901645</v>
+      </c>
+      <c r="Q12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1.755981875366234</v>
+      </c>
+      <c r="T12" t="b">
+        <v>1</v>
+      </c>
+      <c r="U12" t="inlineStr">
         <is>
           <t>Plan downgrade pro-rated refund</t>
         </is>
-      </c>
-      <c r="M12" t="n">
-        <v>3524876.074</v>
-      </c>
-      <c r="N12" t="n">
-        <v>2749486.646</v>
-      </c>
-      <c r="O12" t="n">
-        <v>0.7800236343855077</v>
-      </c>
-      <c r="P12" t="n">
-        <v>3491073.22</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>1.254297556901645</v>
-      </c>
-      <c r="R12" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" t="b">
-        <v>0</v>
-      </c>
-      <c r="T12" t="n">
-        <v>1.755981875366234</v>
-      </c>
-      <c r="U12" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -1341,55 +1345,55 @@
           <t>ACR017</t>
         </is>
       </c>
-      <c r="F13" t="n">
+      <c r="F13" s="2" t="n">
         <v>9812802.08</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13" s="2" t="n">
         <v>9888909.539999999</v>
       </c>
-      <c r="H13" t="n">
+      <c r="H13" s="2" t="n">
         <v>9804506.07</v>
       </c>
-      <c r="I13" t="n">
+      <c r="I13" s="2" t="n">
         <v>10171761.45</v>
       </c>
-      <c r="J13" t="n">
+      <c r="J13" s="2" t="n">
         <v>10326170.02</v>
       </c>
-      <c r="K13" t="n">
+      <c r="K13" s="2" t="n">
         <v>13601635.17</v>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="L13" s="2" t="n">
+        <v>10000829.832</v>
+      </c>
+      <c r="M13" s="2" t="n">
+        <v>3600805.338000001</v>
+      </c>
+      <c r="N13" s="3" t="n">
+        <v>0.3600506556444327</v>
+      </c>
+      <c r="O13" s="2" t="n">
+        <v>3788833.09</v>
+      </c>
+      <c r="P13" s="3" t="n">
+        <v>0.3861112309319093</v>
+      </c>
+      <c r="Q13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" t="b">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>2.517755089011934</v>
+      </c>
+      <c r="T13" t="b">
+        <v>1</v>
+      </c>
+      <c r="U13" t="inlineStr">
         <is>
           <t>Cycle start date adjustment credit</t>
         </is>
-      </c>
-      <c r="M13" t="n">
-        <v>10000829.832</v>
-      </c>
-      <c r="N13" t="n">
-        <v>3600805.338000001</v>
-      </c>
-      <c r="O13" t="n">
-        <v>0.3600506556444327</v>
-      </c>
-      <c r="P13" t="n">
-        <v>3788833.09</v>
-      </c>
-      <c r="Q13" t="n">
-        <v>0.3861112309319093</v>
-      </c>
-      <c r="R13" t="b">
-        <v>0</v>
-      </c>
-      <c r="S13" t="b">
-        <v>0</v>
-      </c>
-      <c r="T13" t="n">
-        <v>2.517755089011934</v>
-      </c>
-      <c r="U13" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -1412,55 +1416,55 @@
           <t>ACR019</t>
         </is>
       </c>
-      <c r="F14" t="n">
+      <c r="F14" s="2" t="n">
         <v>6312462.62</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14" s="2" t="n">
         <v>6220240.08</v>
       </c>
-      <c r="H14" t="n">
+      <c r="H14" s="2" t="n">
         <v>6643218.52</v>
       </c>
-      <c r="I14" t="n">
+      <c r="I14" s="2" t="n">
         <v>6850276.8</v>
       </c>
-      <c r="J14" t="n">
+      <c r="J14" s="2" t="n">
         <v>8075223.11</v>
       </c>
-      <c r="K14" t="n">
+      <c r="K14" s="2" t="n">
         <v>4458212.78</v>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="L14" s="2" t="n">
+        <v>6820284.225999999</v>
+      </c>
+      <c r="M14" s="2" t="n">
+        <v>-2362071.445999999</v>
+      </c>
+      <c r="N14" s="3" t="n">
+        <v>-0.3463303533590887</v>
+      </c>
+      <c r="O14" s="2" t="n">
+        <v>-1854249.84</v>
+      </c>
+      <c r="P14" s="3" t="n">
+        <v>-0.2937442883424156</v>
+      </c>
+      <c r="Q14" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>-2.817919850357314</v>
+      </c>
+      <c r="T14" t="b">
+        <v>1</v>
+      </c>
+      <c r="U14" t="inlineStr">
         <is>
           <t>Tenure loyalty bonus credit</t>
         </is>
-      </c>
-      <c r="M14" t="n">
-        <v>6820284.225999999</v>
-      </c>
-      <c r="N14" t="n">
-        <v>-2362071.445999999</v>
-      </c>
-      <c r="O14" t="n">
-        <v>-0.3463303533590887</v>
-      </c>
-      <c r="P14" t="n">
-        <v>-1854249.84</v>
-      </c>
-      <c r="Q14" t="n">
-        <v>-0.2937442883424156</v>
-      </c>
-      <c r="R14" t="b">
-        <v>0</v>
-      </c>
-      <c r="S14" t="b">
-        <v>0</v>
-      </c>
-      <c r="T14" t="n">
-        <v>-2.817919850357314</v>
-      </c>
-      <c r="U14" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -1483,55 +1487,55 @@
           <t>ACR010</t>
         </is>
       </c>
-      <c r="F15" t="n">
+      <c r="F15" s="2" t="n">
         <v>11824123.94</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15" s="2" t="n">
         <v>12284746.02</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H15" s="2" t="n">
         <v>12225399.82</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I15" s="2" t="n">
         <v>12844480.68</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J15" s="2" t="n">
         <v>14001300.31</v>
       </c>
-      <c r="K15" t="n">
+      <c r="K15" s="2" t="n">
         <v>10223077.64</v>
       </c>
-      <c r="L15" t="inlineStr">
+      <c r="L15" s="2" t="n">
+        <v>12636010.154</v>
+      </c>
+      <c r="M15" s="2" t="n">
+        <v>-2412932.513999999</v>
+      </c>
+      <c r="N15" s="3" t="n">
+        <v>-0.1909568356302857</v>
+      </c>
+      <c r="O15" s="2" t="n">
+        <v>-1601046.299999999</v>
+      </c>
+      <c r="P15" s="3" t="n">
+        <v>-0.13540506748105</v>
+      </c>
+      <c r="Q15" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" t="b">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>-2.863431125493056</v>
+      </c>
+      <c r="T15" t="b">
+        <v>1</v>
+      </c>
+      <c r="U15" t="inlineStr">
         <is>
           <t>Monthly promotional data plan adjustment</t>
         </is>
-      </c>
-      <c r="M15" t="n">
-        <v>12636010.154</v>
-      </c>
-      <c r="N15" t="n">
-        <v>-2412932.513999999</v>
-      </c>
-      <c r="O15" t="n">
-        <v>-0.1909568356302857</v>
-      </c>
-      <c r="P15" t="n">
-        <v>-1601046.299999999</v>
-      </c>
-      <c r="Q15" t="n">
-        <v>-0.13540506748105</v>
-      </c>
-      <c r="R15" t="b">
-        <v>0</v>
-      </c>
-      <c r="S15" t="b">
-        <v>0</v>
-      </c>
-      <c r="T15" t="n">
-        <v>-2.863431125493056</v>
-      </c>
-      <c r="U15" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1554,55 +1558,55 @@
           <t>ACR035</t>
         </is>
       </c>
-      <c r="F16" t="n">
+      <c r="F16" s="2" t="n">
         <v>3945724.03</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16" s="2" t="n">
         <v>4176067.49</v>
       </c>
-      <c r="H16" t="n">
+      <c r="H16" s="2" t="n">
         <v>4401799.99</v>
       </c>
-      <c r="I16" t="n">
+      <c r="I16" s="2" t="n">
         <v>3971431.88</v>
       </c>
-      <c r="J16" t="n">
+      <c r="J16" s="2" t="n">
         <v>4498240.57</v>
       </c>
-      <c r="K16" t="n">
+      <c r="K16" s="2" t="n">
         <v>6340726.7</v>
       </c>
-      <c r="L16" t="inlineStr">
+      <c r="L16" s="2" t="n">
+        <v>4198652.792</v>
+      </c>
+      <c r="M16" s="2" t="n">
+        <v>2142073.908</v>
+      </c>
+      <c r="N16" s="3" t="n">
+        <v>0.5101812448224939</v>
+      </c>
+      <c r="O16" s="2" t="n">
+        <v>2395002.67</v>
+      </c>
+      <c r="P16" s="3" t="n">
+        <v>0.6069868677561823</v>
+      </c>
+      <c r="Q16" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" t="b">
+        <v>0</v>
+      </c>
+      <c r="S16" t="n">
+        <v>1.21245950497337</v>
+      </c>
+      <c r="T16" t="b">
+        <v>1</v>
+      </c>
+      <c r="U16" t="inlineStr">
         <is>
           <t>Plan downgrade pro-rated refund</t>
         </is>
-      </c>
-      <c r="M16" t="n">
-        <v>4198652.792</v>
-      </c>
-      <c r="N16" t="n">
-        <v>2142073.908</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.5101812448224939</v>
-      </c>
-      <c r="P16" t="n">
-        <v>2395002.67</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0.6069868677561823</v>
-      </c>
-      <c r="R16" t="b">
-        <v>0</v>
-      </c>
-      <c r="S16" t="b">
-        <v>0</v>
-      </c>
-      <c r="T16" t="n">
-        <v>1.21245950497337</v>
-      </c>
-      <c r="U16" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -1625,55 +1629,55 @@
           <t>ACR018</t>
         </is>
       </c>
-      <c r="F17" t="n">
+      <c r="F17" s="2" t="n">
         <v>2020462.85</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17" s="2" t="n">
         <v>2089892.97</v>
       </c>
-      <c r="H17" t="n">
+      <c r="H17" s="2" t="n">
         <v>2839030.97</v>
       </c>
-      <c r="I17" t="n">
+      <c r="I17" s="2" t="n">
         <v>2857328.2</v>
       </c>
-      <c r="J17" t="n">
+      <c r="J17" s="2" t="n">
         <v>3687774.15</v>
       </c>
-      <c r="K17" t="n">
+      <c r="K17" s="2" t="n">
         <v>4468377.61</v>
       </c>
-      <c r="L17" t="inlineStr">
+      <c r="L17" s="2" t="n">
+        <v>2698897.828</v>
+      </c>
+      <c r="M17" s="2" t="n">
+        <v>1769479.782</v>
+      </c>
+      <c r="N17" s="3" t="n">
+        <v>0.6556305183702568</v>
+      </c>
+      <c r="O17" s="2" t="n">
+        <v>2447914.76</v>
+      </c>
+      <c r="P17" s="3" t="n">
+        <v>1.21156138060148</v>
+      </c>
+      <c r="Q17" t="b">
+        <v>0</v>
+      </c>
+      <c r="R17" t="b">
+        <v>0</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.8790564827964171</v>
+      </c>
+      <c r="T17" t="b">
+        <v>1</v>
+      </c>
+      <c r="U17" t="inlineStr">
         <is>
           <t>Tax calculation correction credit</t>
         </is>
-      </c>
-      <c r="M17" t="n">
-        <v>2698897.828</v>
-      </c>
-      <c r="N17" t="n">
-        <v>1769479.782</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0.6556305183702568</v>
-      </c>
-      <c r="P17" t="n">
-        <v>2447914.76</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>1.21156138060148</v>
-      </c>
-      <c r="R17" t="b">
-        <v>0</v>
-      </c>
-      <c r="S17" t="b">
-        <v>0</v>
-      </c>
-      <c r="T17" t="n">
-        <v>0.8790564827964171</v>
-      </c>
-      <c r="U17" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="18">
@@ -1696,55 +1700,55 @@
           <t>ACR004</t>
         </is>
       </c>
-      <c r="F18" t="n">
+      <c r="F18" s="2" t="n">
         <v>11003204.71</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18" s="2" t="n">
         <v>11122962.62</v>
       </c>
-      <c r="H18" t="n">
+      <c r="H18" s="2" t="n">
         <v>11845545.08</v>
       </c>
-      <c r="I18" t="n">
+      <c r="I18" s="2" t="n">
         <v>12483149.59</v>
       </c>
-      <c r="J18" t="n">
+      <c r="J18" s="2" t="n">
         <v>12473766.69</v>
       </c>
-      <c r="K18" t="n">
+      <c r="K18" s="2" t="n">
         <v>9670309</v>
       </c>
-      <c r="L18" t="inlineStr">
+      <c r="L18" s="2" t="n">
+        <v>11785725.738</v>
+      </c>
+      <c r="M18" s="2" t="n">
+        <v>-2115416.738</v>
+      </c>
+      <c r="N18" s="3" t="n">
+        <v>-0.1794897306306213</v>
+      </c>
+      <c r="O18" s="2" t="n">
+        <v>-1332895.710000001</v>
+      </c>
+      <c r="P18" s="3" t="n">
+        <v>-0.1211370455362546</v>
+      </c>
+      <c r="Q18" t="b">
+        <v>0</v>
+      </c>
+      <c r="R18" t="b">
+        <v>0</v>
+      </c>
+      <c r="S18" t="n">
+        <v>-2.597209379249744</v>
+      </c>
+      <c r="T18" t="b">
+        <v>1</v>
+      </c>
+      <c r="U18" t="inlineStr">
         <is>
           <t>Loyalty discount applied to account</t>
         </is>
-      </c>
-      <c r="M18" t="n">
-        <v>11785725.738</v>
-      </c>
-      <c r="N18" t="n">
-        <v>-2115416.738</v>
-      </c>
-      <c r="O18" t="n">
-        <v>-0.1794897306306213</v>
-      </c>
-      <c r="P18" t="n">
-        <v>-1332895.710000001</v>
-      </c>
-      <c r="Q18" t="n">
-        <v>-0.1211370455362546</v>
-      </c>
-      <c r="R18" t="b">
-        <v>0</v>
-      </c>
-      <c r="S18" t="b">
-        <v>0</v>
-      </c>
-      <c r="T18" t="n">
-        <v>-2.597209379249744</v>
-      </c>
-      <c r="U18" t="b">
-        <v>1</v>
       </c>
     </row>
     <row r="19">
@@ -1767,52 +1771,52 @@
           <t>SUB008</t>
         </is>
       </c>
-      <c r="F19" t="n">
+      <c r="F19" s="2" t="n">
         <v>10140793.18</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19" s="2" t="n">
         <v>10699154.64</v>
       </c>
-      <c r="H19" t="n">
+      <c r="H19" s="2" t="n">
         <v>10691811.98</v>
       </c>
-      <c r="I19" t="n">
+      <c r="I19" s="2" t="n">
         <v>10705782.79</v>
       </c>
-      <c r="J19" t="n">
+      <c r="J19" s="2" t="n">
         <v>10490837.42</v>
       </c>
-      <c r="K19" t="n">
+      <c r="K19" s="2" t="n">
         <v>14444699.96</v>
       </c>
-      <c r="L19" t="inlineStr"/>
-      <c r="M19" t="n">
+      <c r="L19" s="2" t="n">
         <v>10545676.002</v>
       </c>
-      <c r="N19" t="n">
+      <c r="M19" s="2" t="n">
         <v>3899023.958000001</v>
       </c>
-      <c r="O19" t="n">
+      <c r="N19" s="3" t="n">
         <v>0.3697272661572901</v>
       </c>
-      <c r="P19" t="n">
+      <c r="O19" s="2" t="n">
         <v>4303906.780000001</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="P19" s="3" t="n">
         <v>0.4244152014152409</v>
       </c>
+      <c r="Q19" t="b">
+        <v>0</v>
+      </c>
       <c r="R19" t="b">
         <v>0</v>
       </c>
-      <c r="S19" t="b">
-        <v>0</v>
-      </c>
-      <c r="T19" t="n">
+      <c r="S19" t="n">
         <v>2.784605751003959</v>
       </c>
-      <c r="U19" t="b">
-        <v>1</v>
-      </c>
+      <c r="T19" t="b">
+        <v>1</v>
+      </c>
+      <c r="U19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1834,52 +1838,52 @@
           <t>SUB013</t>
         </is>
       </c>
-      <c r="F20" t="n">
+      <c r="F20" s="2" t="n">
         <v>2480436.38</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20" s="2" t="n">
         <v>2893181.04</v>
       </c>
-      <c r="H20" t="n">
+      <c r="H20" s="2" t="n">
         <v>3076384.69</v>
       </c>
-      <c r="I20" t="n">
+      <c r="I20" s="2" t="n">
         <v>3502157.81</v>
       </c>
-      <c r="J20" t="n">
+      <c r="J20" s="2" t="n">
         <v>3116690.73</v>
       </c>
-      <c r="K20" t="n">
+      <c r="K20" s="2" t="n">
         <v>5300316.99</v>
       </c>
-      <c r="L20" t="inlineStr"/>
-      <c r="M20" t="n">
+      <c r="L20" s="2" t="n">
         <v>3013770.13</v>
       </c>
-      <c r="N20" t="n">
+      <c r="M20" s="2" t="n">
         <v>2286546.86</v>
       </c>
-      <c r="O20" t="n">
+      <c r="N20" s="3" t="n">
         <v>0.7586998216084916</v>
       </c>
-      <c r="P20" t="n">
+      <c r="O20" s="2" t="n">
         <v>2819880.61</v>
       </c>
-      <c r="Q20" t="n">
+      <c r="P20" s="3" t="n">
         <v>1.13684859355272</v>
       </c>
+      <c r="Q20" t="b">
+        <v>0</v>
+      </c>
       <c r="R20" t="b">
         <v>0</v>
       </c>
-      <c r="S20" t="b">
-        <v>0</v>
-      </c>
-      <c r="T20" t="n">
+      <c r="S20" t="n">
         <v>1.341736150680946</v>
       </c>
-      <c r="U20" t="b">
-        <v>1</v>
-      </c>
+      <c r="T20" t="b">
+        <v>1</v>
+      </c>
+      <c r="U20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1901,52 +1905,52 @@
           <t>SUB023</t>
         </is>
       </c>
-      <c r="F21" t="n">
+      <c r="F21" s="2" t="n">
         <v>1416023.85</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21" s="2" t="n">
         <v>2597152.53</v>
       </c>
-      <c r="H21" t="n">
+      <c r="H21" s="2" t="n">
         <v>2451857.32</v>
       </c>
-      <c r="I21" t="n">
+      <c r="I21" s="2" t="n">
         <v>2430676.37</v>
       </c>
-      <c r="J21" t="n">
+      <c r="J21" s="2" t="n">
         <v>2744871.62</v>
       </c>
-      <c r="K21" t="n">
-        <v>0</v>
-      </c>
-      <c r="L21" t="inlineStr"/>
-      <c r="M21" t="n">
+      <c r="K21" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="L21" s="2" t="n">
         <v>2328116.338</v>
       </c>
-      <c r="N21" t="n">
+      <c r="M21" s="2" t="n">
         <v>-2328116.338</v>
       </c>
-      <c r="O21" t="n">
+      <c r="N21" s="3" t="n">
         <v>-1</v>
       </c>
-      <c r="P21" t="n">
+      <c r="O21" s="2" t="n">
         <v>-1416023.85</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="P21" s="3" t="n">
         <v>-1</v>
       </c>
+      <c r="Q21" t="b">
+        <v>1</v>
+      </c>
       <c r="R21" t="b">
-        <v>1</v>
-      </c>
-      <c r="S21" t="b">
-        <v>0</v>
-      </c>
-      <c r="T21" t="n">
+        <v>0</v>
+      </c>
+      <c r="S21" t="n">
         <v>-2.7875362913166</v>
       </c>
-      <c r="U21" t="b">
-        <v>1</v>
-      </c>
+      <c r="T21" t="b">
+        <v>1</v>
+      </c>
+      <c r="U21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1968,52 +1972,52 @@
           <t>SUB033</t>
         </is>
       </c>
-      <c r="F22" t="n">
+      <c r="F22" s="2" t="n">
         <v>2678491.99</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22" s="2" t="n">
         <v>2709952.82</v>
       </c>
-      <c r="H22" t="n">
+      <c r="H22" s="2" t="n">
         <v>3416998.79</v>
       </c>
-      <c r="I22" t="n">
+      <c r="I22" s="2" t="n">
         <v>3171121.65</v>
       </c>
-      <c r="J22" t="n">
+      <c r="J22" s="2" t="n">
         <v>2992346.3</v>
       </c>
-      <c r="K22" t="n">
+      <c r="K22" s="2" t="n">
         <v>4795394.5</v>
       </c>
-      <c r="L22" t="inlineStr"/>
-      <c r="M22" t="n">
+      <c r="L22" s="2" t="n">
         <v>2993782.31</v>
       </c>
-      <c r="N22" t="n">
+      <c r="M22" s="2" t="n">
         <v>1801612.19</v>
       </c>
-      <c r="O22" t="n">
+      <c r="N22" s="3" t="n">
         <v>0.6017846334324825</v>
       </c>
-      <c r="P22" t="n">
+      <c r="O22" s="2" t="n">
         <v>2116902.51</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="P22" s="3" t="n">
         <v>0.7903337093795079</v>
       </c>
+      <c r="Q22" t="b">
+        <v>0</v>
+      </c>
       <c r="R22" t="b">
         <v>0</v>
       </c>
-      <c r="S22" t="b">
-        <v>0</v>
-      </c>
-      <c r="T22" t="n">
+      <c r="S22" t="n">
         <v>0.9078090615126554</v>
       </c>
-      <c r="U22" t="b">
-        <v>1</v>
-      </c>
+      <c r="T22" t="b">
+        <v>1</v>
+      </c>
+      <c r="U22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2035,52 +2039,52 @@
           <t>SUB036</t>
         </is>
       </c>
-      <c r="F23" t="n">
+      <c r="F23" s="2" t="n">
         <v>2637530.04</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23" s="2" t="n">
         <v>2514086.25</v>
       </c>
-      <c r="H23" t="n">
+      <c r="H23" s="2" t="n">
         <v>3585679.69</v>
       </c>
-      <c r="I23" t="n">
+      <c r="I23" s="2" t="n">
         <v>3879506.77</v>
       </c>
-      <c r="J23" t="n">
+      <c r="J23" s="2" t="n">
         <v>3885094.48</v>
       </c>
-      <c r="K23" t="n">
+      <c r="K23" s="2" t="n">
         <v>5913703.08</v>
       </c>
-      <c r="L23" t="inlineStr"/>
-      <c r="M23" t="n">
+      <c r="L23" s="2" t="n">
         <v>3300379.446</v>
       </c>
-      <c r="N23" t="n">
+      <c r="M23" s="2" t="n">
         <v>2613323.634</v>
       </c>
-      <c r="O23" t="n">
+      <c r="N23" s="3" t="n">
         <v>0.7918252057857471</v>
       </c>
-      <c r="P23" t="n">
+      <c r="O23" s="2" t="n">
         <v>3276173.04</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="P23" s="3" t="n">
         <v>1.242136768231842</v>
       </c>
+      <c r="Q23" t="b">
+        <v>0</v>
+      </c>
       <c r="R23" t="b">
         <v>0</v>
       </c>
-      <c r="S23" t="b">
-        <v>0</v>
-      </c>
-      <c r="T23" t="n">
+      <c r="S23" t="n">
         <v>1.634141093288213</v>
       </c>
-      <c r="U23" t="b">
-        <v>1</v>
-      </c>
+      <c r="T23" t="b">
+        <v>1</v>
+      </c>
+      <c r="U23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2102,52 +2106,52 @@
           <t>SUB039</t>
         </is>
       </c>
-      <c r="F24" t="n">
+      <c r="F24" s="2" t="n">
         <v>5769211.05</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24" s="2" t="n">
         <v>5747639.27</v>
       </c>
-      <c r="H24" t="n">
+      <c r="H24" s="2" t="n">
         <v>6007951.66</v>
       </c>
-      <c r="I24" t="n">
+      <c r="I24" s="2" t="n">
         <v>6598640.15</v>
       </c>
-      <c r="J24" t="n">
+      <c r="J24" s="2" t="n">
         <v>6606622.8</v>
       </c>
-      <c r="K24" t="n">
+      <c r="K24" s="2" t="n">
         <v>9648646.24</v>
       </c>
-      <c r="L24" t="inlineStr"/>
-      <c r="M24" t="n">
+      <c r="L24" s="2" t="n">
         <v>6146012.986</v>
       </c>
-      <c r="N24" t="n">
+      <c r="M24" s="2" t="n">
         <v>3502633.254000001</v>
       </c>
-      <c r="O24" t="n">
+      <c r="N24" s="3" t="n">
         <v>0.5699033278938147</v>
       </c>
-      <c r="P24" t="n">
+      <c r="O24" s="2" t="n">
         <v>3879435.19</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="P24" s="3" t="n">
         <v>0.6724377313254991</v>
       </c>
+      <c r="Q24" t="b">
+        <v>0</v>
+      </c>
       <c r="R24" t="b">
         <v>0</v>
       </c>
-      <c r="S24" t="b">
-        <v>0</v>
-      </c>
-      <c r="T24" t="n">
+      <c r="S24" t="n">
         <v>2.429909180515217</v>
       </c>
-      <c r="U24" t="b">
-        <v>1</v>
-      </c>
+      <c r="T24" t="b">
+        <v>1</v>
+      </c>
+      <c r="U24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2169,52 +2173,52 @@
           <t>SUB040</t>
         </is>
       </c>
-      <c r="F25" t="n">
+      <c r="F25" s="2" t="n">
         <v>2401115.84</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25" s="2" t="n">
         <v>2170044.93</v>
       </c>
-      <c r="H25" t="n">
+      <c r="H25" s="2" t="n">
         <v>2524547.49</v>
       </c>
-      <c r="I25" t="n">
+      <c r="I25" s="2" t="n">
         <v>2921294.51</v>
       </c>
-      <c r="J25" t="n">
+      <c r="J25" s="2" t="n">
         <v>2979390.31</v>
       </c>
-      <c r="K25" t="n">
+      <c r="K25" s="2" t="n">
         <v>1027050.36</v>
       </c>
-      <c r="L25" t="inlineStr"/>
-      <c r="M25" t="n">
+      <c r="L25" s="2" t="n">
         <v>2599278.616</v>
       </c>
-      <c r="N25" t="n">
+      <c r="M25" s="2" t="n">
         <v>-1572228.256</v>
       </c>
-      <c r="O25" t="n">
+      <c r="N25" s="3" t="n">
         <v>-0.604871000100591</v>
       </c>
-      <c r="P25" t="n">
+      <c r="O25" s="2" t="n">
         <v>-1374065.48</v>
       </c>
-      <c r="Q25" t="n">
+      <c r="P25" s="3" t="n">
         <v>-0.5722612200167736</v>
       </c>
+      <c r="Q25" t="b">
+        <v>0</v>
+      </c>
       <c r="R25" t="b">
         <v>0</v>
       </c>
-      <c r="S25" t="b">
-        <v>0</v>
-      </c>
-      <c r="T25" t="n">
+      <c r="S25" t="n">
         <v>-2.11115587257017</v>
       </c>
-      <c r="U25" t="b">
-        <v>1</v>
-      </c>
+      <c r="T25" t="b">
+        <v>1</v>
+      </c>
+      <c r="U25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2236,52 +2240,52 @@
           <t>SUB049</t>
         </is>
       </c>
-      <c r="F26" t="n">
+      <c r="F26" s="2" t="n">
         <v>8152951.94</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26" s="2" t="n">
         <v>7952935.3</v>
       </c>
-      <c r="H26" t="n">
+      <c r="H26" s="2" t="n">
         <v>8303657.02</v>
       </c>
-      <c r="I26" t="n">
+      <c r="I26" s="2" t="n">
         <v>9327027.9</v>
       </c>
-      <c r="J26" t="n">
+      <c r="J26" s="2" t="n">
         <v>8912637.779999999</v>
       </c>
-      <c r="K26" t="n">
+      <c r="K26" s="2" t="n">
         <v>12214342.48</v>
       </c>
-      <c r="L26" t="inlineStr"/>
-      <c r="M26" t="n">
+      <c r="L26" s="2" t="n">
         <v>8529841.988</v>
       </c>
-      <c r="N26" t="n">
+      <c r="M26" s="2" t="n">
         <v>3684500.492000001</v>
       </c>
-      <c r="O26" t="n">
+      <c r="N26" s="3" t="n">
         <v>0.4319541319972223</v>
       </c>
-      <c r="P26" t="n">
+      <c r="O26" s="2" t="n">
         <v>4061390.54</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="P26" s="3" t="n">
         <v>0.4981496971758183</v>
       </c>
+      <c r="Q26" t="b">
+        <v>0</v>
+      </c>
       <c r="R26" t="b">
         <v>0</v>
       </c>
-      <c r="S26" t="b">
-        <v>0</v>
-      </c>
-      <c r="T26" t="n">
+      <c r="S26" t="n">
         <v>2.59264681525768</v>
       </c>
-      <c r="U26" t="b">
-        <v>1</v>
-      </c>
+      <c r="T26" t="b">
+        <v>1</v>
+      </c>
+      <c r="U26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2303,52 +2307,52 @@
           <t>SUB063</t>
         </is>
       </c>
-      <c r="F27" t="n">
+      <c r="F27" s="2" t="n">
         <v>3351530.52</v>
       </c>
-      <c r="G27" t="n">
+      <c r="G27" s="2" t="n">
         <v>3743540.81</v>
       </c>
-      <c r="H27" t="n">
+      <c r="H27" s="2" t="n">
         <v>4115479.89</v>
       </c>
-      <c r="I27" t="n">
+      <c r="I27" s="2" t="n">
         <v>4060622.82</v>
       </c>
-      <c r="J27" t="n">
+      <c r="J27" s="2" t="n">
         <v>3758005.4</v>
       </c>
-      <c r="K27" t="n">
+      <c r="K27" s="2" t="n">
         <v>6357218.68</v>
       </c>
-      <c r="L27" t="inlineStr"/>
-      <c r="M27" t="n">
+      <c r="L27" s="2" t="n">
         <v>3805835.888</v>
       </c>
-      <c r="N27" t="n">
+      <c r="M27" s="2" t="n">
         <v>2551382.791999999</v>
       </c>
-      <c r="O27" t="n">
+      <c r="N27" s="3" t="n">
         <v>0.6703869707163788</v>
       </c>
-      <c r="P27" t="n">
+      <c r="O27" s="2" t="n">
         <v>3005688.16</v>
       </c>
-      <c r="Q27" t="n">
+      <c r="P27" s="3" t="n">
         <v>0.896810618928811</v>
       </c>
+      <c r="Q27" t="b">
+        <v>0</v>
+      </c>
       <c r="R27" t="b">
         <v>0</v>
       </c>
-      <c r="S27" t="b">
-        <v>0</v>
-      </c>
-      <c r="T27" t="n">
+      <c r="S27" t="n">
         <v>1.578715463956136</v>
       </c>
-      <c r="U27" t="b">
-        <v>1</v>
-      </c>
+      <c r="T27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2370,52 +2374,52 @@
           <t>SUB092</t>
         </is>
       </c>
-      <c r="F28" t="n">
+      <c r="F28" s="2" t="n">
         <v>4982003.03</v>
       </c>
-      <c r="G28" t="n">
+      <c r="G28" s="2" t="n">
         <v>4701601.07</v>
       </c>
-      <c r="H28" t="n">
+      <c r="H28" s="2" t="n">
         <v>5279670.36</v>
       </c>
-      <c r="I28" t="n">
+      <c r="I28" s="2" t="n">
         <v>5257564.43</v>
       </c>
-      <c r="J28" t="n">
+      <c r="J28" s="2" t="n">
         <v>5527269.71</v>
       </c>
-      <c r="K28" t="n">
+      <c r="K28" s="2" t="n">
         <v>7997910.14</v>
       </c>
-      <c r="L28" t="inlineStr"/>
-      <c r="M28" t="n">
+      <c r="L28" s="2" t="n">
         <v>5149621.720000001</v>
       </c>
-      <c r="N28" t="n">
+      <c r="M28" s="2" t="n">
         <v>2848288.419999999</v>
       </c>
-      <c r="O28" t="n">
+      <c r="N28" s="3" t="n">
         <v>0.5531063396244955</v>
       </c>
-      <c r="P28" t="n">
+      <c r="O28" s="2" t="n">
         <v>3015907.109999999</v>
       </c>
-      <c r="Q28" t="n">
+      <c r="P28" s="3" t="n">
         <v>0.6053603524203395</v>
       </c>
+      <c r="Q28" t="b">
+        <v>0</v>
+      </c>
       <c r="R28" t="b">
         <v>0</v>
       </c>
-      <c r="S28" t="b">
-        <v>0</v>
-      </c>
-      <c r="T28" t="n">
+      <c r="S28" t="n">
         <v>1.844391240274053</v>
       </c>
-      <c r="U28" t="b">
-        <v>1</v>
-      </c>
+      <c r="T28" t="b">
+        <v>1</v>
+      </c>
+      <c r="U28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2437,52 +2441,52 @@
           <t>SUB125</t>
         </is>
       </c>
-      <c r="F29" t="n">
+      <c r="F29" s="2" t="n">
         <v>5802224.63</v>
       </c>
-      <c r="G29" t="n">
+      <c r="G29" s="2" t="n">
         <v>6076078.32</v>
       </c>
-      <c r="H29" t="n">
+      <c r="H29" s="2" t="n">
         <v>6247691.02</v>
       </c>
-      <c r="I29" t="n">
+      <c r="I29" s="2" t="n">
         <v>6779083.83</v>
       </c>
-      <c r="J29" t="n">
+      <c r="J29" s="2" t="n">
         <v>5533459.32</v>
       </c>
-      <c r="K29" t="n">
+      <c r="K29" s="2" t="n">
         <v>9299769.25</v>
       </c>
-      <c r="L29" t="inlineStr"/>
-      <c r="M29" t="n">
+      <c r="L29" s="2" t="n">
         <v>6087707.424000001</v>
       </c>
-      <c r="N29" t="n">
+      <c r="M29" s="2" t="n">
         <v>3212061.825999999</v>
       </c>
-      <c r="O29" t="n">
+      <c r="N29" s="3" t="n">
         <v>0.5276307815544585</v>
       </c>
-      <c r="P29" t="n">
+      <c r="O29" s="2" t="n">
         <v>3497544.62</v>
       </c>
-      <c r="Q29" t="n">
+      <c r="P29" s="3" t="n">
         <v>0.6027937287908828</v>
       </c>
+      <c r="Q29" t="b">
+        <v>0</v>
+      </c>
       <c r="R29" t="b">
         <v>0</v>
       </c>
-      <c r="S29" t="b">
-        <v>0</v>
-      </c>
-      <c r="T29" t="n">
+      <c r="S29" t="n">
         <v>2.169901344928799</v>
       </c>
-      <c r="U29" t="b">
-        <v>1</v>
-      </c>
+      <c r="T29" t="b">
+        <v>1</v>
+      </c>
+      <c r="U29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2504,52 +2508,52 @@
           <t>SUB142</t>
         </is>
       </c>
-      <c r="F30" t="n">
+      <c r="F30" s="2" t="n">
         <v>1099090.88</v>
       </c>
-      <c r="G30" t="n">
+      <c r="G30" s="2" t="n">
         <v>1183423.86</v>
       </c>
-      <c r="H30" t="n">
+      <c r="H30" s="2" t="n">
         <v>2005760.04</v>
       </c>
-      <c r="I30" t="n">
+      <c r="I30" s="2" t="n">
         <v>2079038.2</v>
       </c>
-      <c r="J30" t="n">
+      <c r="J30" s="2" t="n">
         <v>2810409.55</v>
       </c>
-      <c r="K30" t="n">
+      <c r="K30" s="2" t="n">
         <v>3215916.01</v>
       </c>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="n">
+      <c r="L30" s="2" t="n">
         <v>1835544.506</v>
       </c>
-      <c r="N30" t="n">
+      <c r="M30" s="2" t="n">
         <v>1380371.503999999</v>
       </c>
-      <c r="O30" t="n">
+      <c r="N30" s="3" t="n">
         <v>0.7520229008274448</v>
       </c>
-      <c r="P30" t="n">
+      <c r="O30" s="2" t="n">
         <v>2116825.13</v>
       </c>
-      <c r="Q30" t="n">
+      <c r="P30" s="3" t="n">
         <v>1.925978250315388</v>
       </c>
+      <c r="Q30" t="b">
+        <v>0</v>
+      </c>
       <c r="R30" t="b">
         <v>0</v>
       </c>
-      <c r="S30" t="b">
-        <v>0</v>
-      </c>
-      <c r="T30" t="n">
+      <c r="S30" t="n">
         <v>0.5308763404200716</v>
       </c>
-      <c r="U30" t="b">
-        <v>1</v>
-      </c>
+      <c r="T30" t="b">
+        <v>1</v>
+      </c>
+      <c r="U30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2571,52 +2575,52 @@
           <t>SUB145</t>
         </is>
       </c>
-      <c r="F31" t="n">
+      <c r="F31" s="2" t="n">
         <v>1091372.52</v>
       </c>
-      <c r="G31" t="n">
+      <c r="G31" s="2" t="n">
         <v>1791003.69</v>
       </c>
-      <c r="H31" t="n">
+      <c r="H31" s="2" t="n">
         <v>1863793.89</v>
       </c>
-      <c r="I31" t="n">
+      <c r="I31" s="2" t="n">
         <v>2528651.14</v>
       </c>
-      <c r="J31" t="n">
+      <c r="J31" s="2" t="n">
         <v>2976744.97</v>
       </c>
-      <c r="K31" t="n">
+      <c r="K31" s="2" t="n">
         <v>3834339.96</v>
       </c>
-      <c r="L31" t="inlineStr"/>
-      <c r="M31" t="n">
+      <c r="L31" s="2" t="n">
         <v>2050313.242</v>
       </c>
-      <c r="N31" t="n">
+      <c r="M31" s="2" t="n">
         <v>1784026.718</v>
       </c>
-      <c r="O31" t="n">
+      <c r="N31" s="3" t="n">
         <v>0.8701239798167387</v>
       </c>
-      <c r="P31" t="n">
+      <c r="O31" s="2" t="n">
         <v>2742967.44</v>
       </c>
-      <c r="Q31" t="n">
+      <c r="P31" s="3" t="n">
         <v>2.513319136897454</v>
       </c>
+      <c r="Q31" t="b">
+        <v>0</v>
+      </c>
       <c r="R31" t="b">
         <v>0</v>
       </c>
-      <c r="S31" t="b">
-        <v>0</v>
-      </c>
-      <c r="T31" t="n">
+      <c r="S31" t="n">
         <v>0.8920733075056041</v>
       </c>
-      <c r="U31" t="b">
-        <v>1</v>
-      </c>
+      <c r="T31" t="b">
+        <v>1</v>
+      </c>
+      <c r="U31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2638,52 +2642,52 @@
           <t>ADD043</t>
         </is>
       </c>
-      <c r="F32" t="n">
+      <c r="F32" s="2" t="n">
         <v>1348306.51</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G32" s="2" t="n">
         <v>1632505.7</v>
       </c>
-      <c r="H32" t="n">
+      <c r="H32" s="2" t="n">
         <v>2392801.45</v>
       </c>
-      <c r="I32" t="n">
+      <c r="I32" s="2" t="n">
         <v>2676634.31</v>
       </c>
-      <c r="J32" t="n">
+      <c r="J32" s="2" t="n">
         <v>2203788.7</v>
       </c>
-      <c r="K32" t="n">
+      <c r="K32" s="2" t="n">
         <v>4951676.74</v>
       </c>
-      <c r="L32" t="inlineStr"/>
-      <c r="M32" t="n">
+      <c r="L32" s="2" t="n">
         <v>2050807.334</v>
       </c>
-      <c r="N32" t="n">
+      <c r="M32" s="2" t="n">
         <v>2900869.406</v>
       </c>
-      <c r="O32" t="n">
+      <c r="N32" s="3" t="n">
         <v>1.414501185902235</v>
       </c>
-      <c r="P32" t="n">
+      <c r="O32" s="2" t="n">
         <v>3603370.23</v>
       </c>
-      <c r="Q32" t="n">
+      <c r="P32" s="3" t="n">
         <v>2.672515635929104</v>
       </c>
+      <c r="Q32" t="b">
+        <v>0</v>
+      </c>
       <c r="R32" t="b">
         <v>0</v>
       </c>
-      <c r="S32" t="b">
-        <v>0</v>
-      </c>
-      <c r="T32" t="n">
+      <c r="S32" t="n">
         <v>1.891441524801202</v>
       </c>
-      <c r="U32" t="b">
-        <v>1</v>
-      </c>
+      <c r="T32" t="b">
+        <v>1</v>
+      </c>
+      <c r="U32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2705,52 +2709,52 @@
           <t>ADD049</t>
         </is>
       </c>
-      <c r="F33" t="n">
+      <c r="F33" s="2" t="n">
         <v>3579886.93</v>
       </c>
-      <c r="G33" t="n">
+      <c r="G33" s="2" t="n">
         <v>4611467.52</v>
       </c>
-      <c r="H33" t="n">
+      <c r="H33" s="2" t="n">
         <v>4522842.25</v>
       </c>
-      <c r="I33" t="n">
+      <c r="I33" s="2" t="n">
         <v>4470433.61</v>
       </c>
-      <c r="J33" t="n">
+      <c r="J33" s="2" t="n">
         <v>4651892.37</v>
       </c>
-      <c r="K33" t="n">
+      <c r="K33" s="2" t="n">
         <v>8715758.300000001</v>
       </c>
-      <c r="L33" t="inlineStr"/>
-      <c r="M33" t="n">
+      <c r="L33" s="2" t="n">
         <v>4367304.536</v>
       </c>
-      <c r="N33" t="n">
+      <c r="M33" s="2" t="n">
         <v>4348453.764</v>
       </c>
-      <c r="O33" t="n">
+      <c r="N33" s="3" t="n">
         <v>0.9956836598307693</v>
       </c>
-      <c r="P33" t="n">
+      <c r="O33" s="2" t="n">
         <v>5135871.370000001</v>
       </c>
-      <c r="Q33" t="n">
+      <c r="P33" s="3" t="n">
         <v>1.434646252919502</v>
       </c>
+      <c r="Q33" t="b">
+        <v>0</v>
+      </c>
       <c r="R33" t="b">
         <v>0</v>
       </c>
-      <c r="S33" t="b">
-        <v>0</v>
-      </c>
-      <c r="T33" t="n">
+      <c r="S33" t="n">
         <v>3.186762535345753</v>
       </c>
-      <c r="U33" t="b">
-        <v>1</v>
-      </c>
+      <c r="T33" t="b">
+        <v>1</v>
+      </c>
+      <c r="U33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2772,52 +2776,52 @@
           <t>ADD084</t>
         </is>
       </c>
-      <c r="F34" t="n">
+      <c r="F34" s="2" t="n">
         <v>1450140.72</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G34" s="2" t="n">
         <v>1719533.1</v>
       </c>
-      <c r="H34" t="n">
+      <c r="H34" s="2" t="n">
         <v>1653116.69</v>
       </c>
-      <c r="I34" t="n">
+      <c r="I34" s="2" t="n">
         <v>1906944.4</v>
       </c>
-      <c r="J34" t="n">
+      <c r="J34" s="2" t="n">
         <v>3217877.6</v>
       </c>
-      <c r="K34" t="n">
+      <c r="K34" s="2" t="n">
         <v>3212586.14</v>
       </c>
-      <c r="L34" t="inlineStr"/>
-      <c r="M34" t="n">
+      <c r="L34" s="2" t="n">
         <v>1989522.502</v>
       </c>
-      <c r="N34" t="n">
+      <c r="M34" s="2" t="n">
         <v>1223063.638</v>
       </c>
-      <c r="O34" t="n">
+      <c r="N34" s="3" t="n">
         <v>0.614752352270706</v>
       </c>
-      <c r="P34" t="n">
+      <c r="O34" s="2" t="n">
         <v>1762445.42</v>
       </c>
-      <c r="Q34" t="n">
+      <c r="P34" s="3" t="n">
         <v>1.215361651247198</v>
       </c>
+      <c r="Q34" t="b">
+        <v>0</v>
+      </c>
       <c r="R34" t="b">
         <v>0</v>
       </c>
-      <c r="S34" t="b">
-        <v>0</v>
-      </c>
-      <c r="T34" t="n">
+      <c r="S34" t="n">
         <v>0.3901148139310393</v>
       </c>
-      <c r="U34" t="b">
-        <v>1</v>
-      </c>
+      <c r="T34" t="b">
+        <v>1</v>
+      </c>
+      <c r="U34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>